<commit_message>
updated bio text to center
</commit_message>
<xml_diff>
--- a/data-raw/navlinks.xlsx
+++ b/data-raw/navlinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\ACCESSLandingPage\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF11EA0E-CA32-4F82-839D-ACC496ED55CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE16AC7-D0A5-43E8-96D2-78817F464764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3005" yWindow="-10890" windowWidth="19380" windowHeight="10260" xr2:uid="{C2DDE7F5-3915-430B-BDDB-1BA09EB881D0}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
New button text in data
</commit_message>
<xml_diff>
--- a/data-raw/navlinks.xlsx
+++ b/data-raw/navlinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\ACCESSLandingPage\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0503F1A8-3C2B-460D-85DC-4F61615B6D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A4BFE6-3185-46E7-84DF-54A98EFE611B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C2DDE7F5-3915-430B-BDDB-1BA09EB881D0}"/>
+    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" xr2:uid="{C2DDE7F5-3915-430B-BDDB-1BA09EB881D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>https://calendly.com/mdmccarthy/navigatorappt</t>
   </si>
@@ -182,6 +182,33 @@
 Chioma has a wide range of research interests, such as the impact of restrictive gender roles on self-actualization, hustle culture's impact on dimensions of self-care, and cultural retention among Igbo/African immigrants in the United States. 
 Chioma promotes her well-being through creative writing, music, socializing and engaging in new experiences. 
 Pronouns: She/her/hers </t>
+  </si>
+  <si>
+    <t>Mikhaela</t>
+  </si>
+  <si>
+    <t>Chioma</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>Shea</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Shortname</t>
+  </si>
+  <si>
+    <t>Meg</t>
   </si>
 </sst>
 </file>
@@ -232,11 +259,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA84693-C709-49D2-A664-53B525EE7781}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +609,7 @@
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -596,8 +622,11 @@
       <c r="D1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -607,11 +636,14 @@
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -624,8 +656,11 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -635,11 +670,14 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -649,11 +687,14 @@
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -666,8 +707,11 @@
       <c r="D6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -677,11 +721,14 @@
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -694,8 +741,11 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -705,11 +755,14 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>

</xml_diff>